<commit_message>
create fertilizer insert initialization data script
</commit_message>
<xml_diff>
--- a/database/schemas.xlsx
+++ b/database/schemas.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\桌面\SQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A04F0B9-1187-43DD-A7EF-8379E9B1E22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F7BFA9-AE34-4187-94A2-D63AE3F1AA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{739AC6C9-781D-4800-890D-3948D11B4BA9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{739AC6C9-781D-4800-890D-3948D11B4BA9}"/>
   </bookViews>
   <sheets>
     <sheet name="product_imformation" sheetId="1" r:id="rId1"/>
     <sheet name="fertilizer" sheetId="2" r:id="rId2"/>
-    <sheet name="sensor_data" sheetId="3" r:id="rId3"/>
+    <sheet name="pesticide" sheetId="5" r:id="rId3"/>
+    <sheet name="CH4_sensor_data" sheetId="3" r:id="rId4"/>
+    <sheet name="CO2_sensor_data" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
   <si>
     <t>ppm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -85,10 +87,6 @@
   </si>
   <si>
     <t>K2O_kg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>農藥肥料名稱</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -108,45 +106,108 @@
 公斤</t>
   </si>
   <si>
+    <t>final_co2e</t>
+  </si>
+  <si>
+    <t>grow_crops</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>種植的農作物</t>
+  </si>
+  <si>
+    <t>總CO2E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>肥料名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>農藥名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用的農藥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用的肥料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pesticide</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>農藥的劑量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>肥料的劑量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dosage_fertilizer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dosage_pesticide</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>co2e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>creater</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>area</t>
-  </si>
-  <si>
-    <t>Fertilizer</t>
-  </si>
-  <si>
-    <t>dosage</t>
-  </si>
-  <si>
-    <t>Fertilizer_co2e</t>
-  </si>
-  <si>
-    <t>final_co2e</t>
-  </si>
-  <si>
-    <t>grow_crops</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>種植的農作物</t>
-  </si>
-  <si>
-    <t>種植區域</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用的農藥肥料</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>農藥肥料的劑量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用的農藥肥料所產生的CO2E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>總CO2E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>產地</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">origin_place </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>種植面積</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>農友(輸入者)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fertilizer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用的肥料所產生的CO2E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用的農藥所產生的CO2E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fertilizer_co2e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pesticide_co2e</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -533,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{432F3A33-A0CD-4FB1-BD88-33919A611198}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -548,13 +609,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -562,54 +623,109 @@
         <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>18</v>
+      <c r="A3" t="s">
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -620,10 +736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF759011-DD42-4496-89DC-C909A4C52BC5}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -641,7 +757,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -652,7 +768,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -663,7 +779,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -674,7 +790,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -685,7 +801,18 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -695,17 +822,72 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE39D71-4AB2-4083-82D8-C3FA2C12C34B}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6116031A-0DEF-4B18-9193-48F901230846}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE39D71-4AB2-4083-82D8-C3FA2C12C34B}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
     <col min="3" max="3" width="33.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -735,4 +917,47 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB85FAE3-EAAB-4178-975A-2D92CB0588F0}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>